<commit_message>
Update ICS Summary to include 2024
</commit_message>
<xml_diff>
--- a/LakeMeadWaterConservationProgramAnalysis/LakeMeadStorageICS/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/LakeMeadWaterConservationProgramAnalysis/LakeMeadStorageICS/IntentionallyCreatedSurplus-Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\ICS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterConservationProgramAnalysis\LakeMeadStorageICS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACF12E2-AA49-4594-8D0D-8D62EF378416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375BD56C-463E-4677-BAC7-822E220F92CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="6" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="79">
   <si>
     <t>Data Sources:</t>
   </si>
@@ -298,6 +298,9 @@
   </si>
   <si>
     <t>Account balance by state and contractor</t>
+  </si>
+  <si>
+    <t>Balance - Dec 2024 (AF)</t>
   </si>
 </sst>
 </file>
@@ -735,7 +738,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -828,13 +831,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -920,7 +923,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F18" si="1">SUM(B3:D3)</f>
+        <f t="shared" ref="F3:F19" si="1">SUM(B3:D3)</f>
         <v>593573</v>
       </c>
       <c r="G3" s="10">
@@ -1389,6 +1392,35 @@
       <c r="H18" s="11">
         <f>SUM(E18:F18)</f>
         <v>3538939</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="16">
+        <v>710589</v>
+      </c>
+      <c r="C19" s="16">
+        <v>1661832</v>
+      </c>
+      <c r="D19" s="16">
+        <v>954013</v>
+      </c>
+      <c r="E19" s="11">
+        <f>E18+30000</f>
+        <v>240975</v>
+      </c>
+      <c r="F19" s="2">
+        <f t="shared" si="1"/>
+        <v>3326434</v>
+      </c>
+      <c r="G19" s="12">
+        <v>2024</v>
+      </c>
+      <c r="H19" s="11">
+        <f>SUM(E19:F19)</f>
+        <v>3567409</v>
       </c>
     </row>
   </sheetData>
@@ -1401,10 +1433,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83C452AE-E84E-4682-A6B7-6BBA39D2CE31}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B18" sqref="B18:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1877,6 +1909,31 @@
       <c r="F18" s="16">
         <f>Balances!E18-Balances!E17</f>
         <v>-34000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="12">
+        <v>2024</v>
+      </c>
+      <c r="B19" s="16">
+        <f t="shared" ref="B19" si="1">SUM(C19:F19)</f>
+        <v>28470</v>
+      </c>
+      <c r="C19" s="16">
+        <f>Balances!B19-Balances!B18</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="16">
+        <f>Balances!C19-Balances!C18</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="16">
+        <f>Balances!D19-Balances!D18</f>
+        <v>-1530</v>
+      </c>
+      <c r="F19" s="16">
+        <f>Balances!E19-Balances!E18</f>
+        <v>30000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>